<commit_message>
March to June Added!!
</commit_message>
<xml_diff>
--- a/2021-2022/10-March/March Report.xlsx
+++ b/2021-2022/10-March/March Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Bhuvnesh\Hetal Ben\2021-2022\10-March\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93E8C9A-B9A2-418B-935D-30CC68EA217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26EF78E-1BAC-4EBA-9D0A-8E9E7B750C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,6 +1042,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1057,43 +1094,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1122,6 +1122,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1138,24 +1156,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1378,8 +1378,8 @@
   </sheetPr>
   <dimension ref="A1:AF1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22:Y39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1411,236 +1411,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="87"/>
+      <c r="A1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="88"/>
     </row>
     <row r="2" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A2" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="75"/>
+      <c r="A2" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="79"/>
     </row>
     <row r="3" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="78"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81"/>
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="81"/>
+      <c r="W3" s="81"/>
+      <c r="X3" s="81"/>
+      <c r="Y3" s="82"/>
     </row>
     <row r="4" spans="1:29" ht="19.5" customHeight="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="81"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="84"/>
+      <c r="X4" s="84"/>
+      <c r="Y4" s="85"/>
     </row>
     <row r="5" spans="1:29" ht="19.5" customHeight="1">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="83"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="84"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="73"/>
+      <c r="W5" s="73"/>
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74"/>
     </row>
     <row r="6" spans="1:29" ht="19.5" customHeight="1">
       <c r="A6" s="39"/>
-      <c r="B6" s="82" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="82" t="s">
+      <c r="B6" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="82" t="s">
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="84"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="73"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
+      <c r="X6" s="73"/>
+      <c r="Y6" s="74"/>
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="37.5" customHeight="1">
       <c r="A7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="92" t="s">
+      <c r="C7" s="76"/>
+      <c r="D7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="92" t="s">
+      <c r="E7" s="76"/>
+      <c r="F7" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="93"/>
-      <c r="H7" s="88" t="s">
+      <c r="G7" s="76"/>
+      <c r="H7" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="89"/>
-      <c r="J7" s="92" t="s">
+      <c r="I7" s="69"/>
+      <c r="J7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="93"/>
-      <c r="L7" s="92" t="s">
+      <c r="K7" s="76"/>
+      <c r="L7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="93"/>
-      <c r="N7" s="92" t="s">
+      <c r="M7" s="76"/>
+      <c r="N7" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="93"/>
-      <c r="P7" s="88" t="s">
+      <c r="O7" s="76"/>
+      <c r="P7" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="89"/>
-      <c r="R7" s="90" t="s">
+      <c r="Q7" s="69"/>
+      <c r="R7" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="91"/>
-      <c r="T7" s="90" t="s">
+      <c r="S7" s="71"/>
+      <c r="T7" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="91"/>
-      <c r="V7" s="90" t="s">
+      <c r="U7" s="71"/>
+      <c r="V7" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="W7" s="91"/>
-      <c r="X7" s="88" t="s">
+      <c r="W7" s="71"/>
+      <c r="X7" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="Y7" s="89"/>
+      <c r="Y7" s="69"/>
       <c r="Z7" s="1"/>
       <c r="AA7" t="s">
         <v>119</v>
@@ -1845,11 +1845,11 @@
         <v>0</v>
       </c>
       <c r="H10" s="46">
-        <f t="shared" ref="H10:H34" si="1">SUM(B10+D10+F10)</f>
+        <f t="shared" ref="H10:H22" si="1">SUM(B10+D10+F10)</f>
         <v>0</v>
       </c>
       <c r="I10" s="46">
-        <f t="shared" ref="I10:I34" si="2">SUM(C10+E10+G10)</f>
+        <f t="shared" ref="I10:I22" si="2">SUM(C10+E10+G10)</f>
         <v>0</v>
       </c>
       <c r="J10" s="39">
@@ -1871,11 +1871,11 @@
         <v>0</v>
       </c>
       <c r="P10" s="46">
-        <f t="shared" ref="P10:P34" si="3">SUM(J10+L10+N10)</f>
+        <f t="shared" ref="P10:P22" si="3">SUM(J10+L10+N10)</f>
         <v>0</v>
       </c>
       <c r="Q10" s="46">
-        <f t="shared" ref="Q10:Q34" si="4">SUM(K10+M10+O10)</f>
+        <f t="shared" ref="Q10:Q22" si="4">SUM(K10+M10+O10)</f>
         <v>0</v>
       </c>
       <c r="R10" s="48">
@@ -2194,11 +2194,11 @@
         <v>1</v>
       </c>
       <c r="X13" s="46">
-        <f t="shared" ref="X13:X38" si="13">SUM(R13+T13+V13)</f>
+        <f t="shared" ref="X13:X22" si="13">SUM(R13+T13+V13)</f>
         <v>4</v>
       </c>
       <c r="Y13" s="46">
-        <f t="shared" ref="Y13:Y38" si="14">SUM(S13+U13+W13)</f>
+        <f t="shared" ref="Y13:Y22" si="14">SUM(S13+U13+W13)</f>
         <v>5</v>
       </c>
       <c r="AA13" s="54">
@@ -3137,36 +3137,41 @@
         <v>8</v>
       </c>
       <c r="R23" s="48">
-        <v>0</v>
+        <f t="shared" ref="R23:R39" si="32">SUM(B23+J23)</f>
+        <v>3</v>
       </c>
       <c r="S23" s="48">
-        <v>0</v>
+        <f t="shared" ref="S23:S39" si="33">SUM(C23+K23)</f>
+        <v>2</v>
       </c>
       <c r="T23" s="48">
-        <v>0</v>
+        <f t="shared" ref="T23:T39" si="34">SUM(D23+L23)</f>
+        <v>3</v>
       </c>
       <c r="U23" s="48">
-        <v>0</v>
+        <f t="shared" ref="U23:U39" si="35">SUM(E23+M23)</f>
+        <v>6</v>
       </c>
       <c r="V23" s="48">
+        <f t="shared" ref="V23:V39" si="36">SUM(F23+N23)</f>
         <v>0</v>
       </c>
       <c r="W23" s="48">
-        <f t="shared" ref="W23" si="32">SUM(G23+O23)</f>
+        <f t="shared" ref="W23:W39" si="37">SUM(G23+O23)</f>
         <v>3</v>
       </c>
       <c r="X23" s="46">
-        <f t="shared" ref="X23:X39" si="33">SUM(R23+T23+V23)</f>
-        <v>0</v>
+        <f t="shared" ref="X23:X39" si="38">SUM(R23+T23+V23)</f>
+        <v>6</v>
       </c>
       <c r="Y23" s="46">
-        <f t="shared" ref="Y23:Y39" si="34">SUM(S23+U23+W23)</f>
-        <v>3</v>
+        <f t="shared" ref="Y23:Y39" si="39">SUM(S23+U23+W23)</f>
+        <v>11</v>
       </c>
       <c r="Z23" s="67"/>
       <c r="AA23" s="54">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="AC23" s="55">
         <f t="shared" si="8"/>
@@ -3230,15 +3235,15 @@
         <v>5</v>
       </c>
       <c r="R24" s="48">
-        <f t="shared" ref="R24:W24" si="35">SUM(B24+J24)</f>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="S24" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="T24" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="U24" s="48">
@@ -3246,19 +3251,19 @@
         <v>4</v>
       </c>
       <c r="V24" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3</v>
       </c>
       <c r="W24" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X24" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>10</v>
       </c>
       <c r="Y24" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>6</v>
       </c>
       <c r="AA24" s="54">
@@ -3327,19 +3332,19 @@
         <v>3</v>
       </c>
       <c r="R25" s="48">
-        <f t="shared" ref="R25:W25" si="36">SUM(B25+J25)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="S25" s="48">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="T25" s="48">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>3</v>
       </c>
       <c r="U25" s="48">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="V25" s="48">
@@ -3347,15 +3352,15 @@
         <v>0</v>
       </c>
       <c r="W25" s="48">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="X25" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="Y25" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="AA25" s="54">
@@ -3424,23 +3429,23 @@
         <v>0</v>
       </c>
       <c r="R26" s="48">
-        <f t="shared" ref="R26:W26" si="37">SUM(B26+J26)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S26" s="48">
-        <f t="shared" si="37"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="T26" s="48">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="U26" s="48">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="V26" s="48">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W26" s="48">
@@ -3448,11 +3453,11 @@
         <v>0</v>
       </c>
       <c r="X26" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y26" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA26" s="54">
@@ -3521,35 +3526,35 @@
         <v>3</v>
       </c>
       <c r="R27" s="48">
-        <f t="shared" ref="R27:W27" si="38">SUM(B27+J27)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S27" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="T27" s="48">
+        <f t="shared" si="34"/>
+        <v>3</v>
+      </c>
+      <c r="U27" s="48">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="V27" s="48">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="W27" s="48">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="X27" s="46">
         <f t="shared" si="38"/>
         <v>3</v>
       </c>
-      <c r="U27" s="48">
-        <f t="shared" si="38"/>
-        <v>2</v>
-      </c>
-      <c r="V27" s="48">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="W27" s="48">
-        <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="X27" s="46">
-        <f t="shared" si="33"/>
-        <v>3</v>
-      </c>
       <c r="Y27" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="AA27" s="54">
@@ -3618,29 +3623,35 @@
         <v>0</v>
       </c>
       <c r="R28" s="48">
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S28" s="48">
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="T28" s="48">
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="U28" s="48">
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="V28" s="48">
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W28" s="48">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="X28" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y28" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA28" s="54">
@@ -3709,35 +3720,35 @@
         <v>5</v>
       </c>
       <c r="R29" s="48">
-        <f t="shared" ref="R29:W29" si="39">SUM(B29+J29)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="S29" s="48">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="T29" s="48">
+        <f t="shared" si="34"/>
+        <v>6</v>
+      </c>
+      <c r="U29" s="48">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="V29" s="48">
+        <f t="shared" si="36"/>
+        <v>3</v>
+      </c>
+      <c r="W29" s="48">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="X29" s="46">
+        <f t="shared" si="38"/>
+        <v>10</v>
+      </c>
+      <c r="Y29" s="46">
         <f t="shared" si="39"/>
-        <v>4</v>
-      </c>
-      <c r="T29" s="48">
-        <f t="shared" si="39"/>
-        <v>6</v>
-      </c>
-      <c r="U29" s="48">
-        <f t="shared" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="V29" s="48">
-        <f t="shared" si="39"/>
-        <v>3</v>
-      </c>
-      <c r="W29" s="48">
-        <f t="shared" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="X29" s="46">
-        <f t="shared" si="33"/>
-        <v>10</v>
-      </c>
-      <c r="Y29" s="46">
-        <f t="shared" si="34"/>
         <v>7</v>
       </c>
       <c r="AA29" s="54">
@@ -3806,35 +3817,35 @@
         <v>8</v>
       </c>
       <c r="R30" s="48">
-        <f t="shared" ref="R30:W30" si="40">SUM(B30+J30)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="S30" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="T30" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="U30" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>8</v>
       </c>
       <c r="V30" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W30" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X30" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>5</v>
       </c>
       <c r="Y30" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>11</v>
       </c>
       <c r="AA30" s="54">
@@ -3903,35 +3914,35 @@
         <v>5</v>
       </c>
       <c r="R31" s="48">
-        <f t="shared" ref="R31:W31" si="41">SUM(B31+J31)</f>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="S31" s="48">
-        <f t="shared" si="41"/>
+        <f t="shared" si="33"/>
         <v>3</v>
       </c>
       <c r="T31" s="48">
-        <f t="shared" si="41"/>
+        <f t="shared" si="34"/>
         <v>3</v>
       </c>
       <c r="U31" s="48">
-        <f t="shared" si="41"/>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="V31" s="48">
-        <f t="shared" si="41"/>
+        <f t="shared" si="36"/>
         <v>3</v>
       </c>
       <c r="W31" s="48">
-        <f t="shared" si="41"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X31" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>11</v>
       </c>
       <c r="Y31" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
       <c r="AA31" s="54">
@@ -4000,35 +4011,35 @@
         <v>4</v>
       </c>
       <c r="R32" s="48">
-        <f t="shared" ref="R32:W32" si="42">SUM(B32+J32)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="S32" s="48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="T32" s="48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="U32" s="48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="V32" s="48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="36"/>
         <v>3</v>
       </c>
       <c r="W32" s="48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X32" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>9</v>
       </c>
       <c r="Y32" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>6</v>
       </c>
       <c r="AA32" s="54">
@@ -4097,35 +4108,35 @@
         <v>8</v>
       </c>
       <c r="R33" s="48">
-        <f t="shared" ref="R33:W33" si="43">SUM(B33+J33)</f>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="S33" s="48">
-        <f t="shared" si="43"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="T33" s="48">
-        <f t="shared" si="43"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="U33" s="48">
-        <f t="shared" si="43"/>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="V33" s="48">
-        <f t="shared" si="43"/>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="W33" s="48">
-        <f t="shared" si="43"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="X33" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="Y33" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>12</v>
       </c>
       <c r="AA33" s="54">
@@ -4194,35 +4205,35 @@
         <v>1</v>
       </c>
       <c r="R34" s="48">
-        <f t="shared" ref="R34:W34" si="44">SUM(B34+J34)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="S34" s="48">
-        <f t="shared" si="44"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="T34" s="48">
-        <f t="shared" si="44"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="U34" s="48">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
       <c r="V34" s="48">
-        <f>SUM(F34+N34)</f>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="W34" s="48">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X34" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>6</v>
       </c>
       <c r="Y34" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="AA34" s="54">
@@ -4291,35 +4302,35 @@
         <v>0</v>
       </c>
       <c r="R35" s="48">
-        <f t="shared" ref="R35:R39" si="45">SUM(B35+J35)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S35" s="48">
-        <f t="shared" ref="S35:S39" si="46">SUM(C35+K35)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="T35" s="48">
-        <f t="shared" ref="T35:T39" si="47">SUM(D35+L35)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="U35" s="48">
-        <f t="shared" ref="U35:U39" si="48">SUM(E35+M35)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="V35" s="48">
-        <f t="shared" ref="V35:V39" si="49">SUM(F35+N35)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W35" s="48">
-        <f t="shared" ref="W35:W39" si="50">SUM(G35+O35)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="X35" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y35" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA35" s="54">
@@ -4388,35 +4399,35 @@
         <v>5</v>
       </c>
       <c r="R36" s="48">
-        <f t="shared" si="45"/>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="S36" s="48">
-        <f t="shared" si="46"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="T36" s="48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="U36" s="48">
-        <f t="shared" si="48"/>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="V36" s="48">
-        <f t="shared" si="49"/>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="W36" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X36" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>12</v>
       </c>
       <c r="Y36" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
       <c r="AA36" s="54">
@@ -4485,35 +4496,35 @@
         <v>6</v>
       </c>
       <c r="R37" s="48">
-        <f t="shared" si="45"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="S37" s="48">
-        <f t="shared" si="46"/>
+        <f t="shared" si="33"/>
         <v>4</v>
       </c>
       <c r="T37" s="48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="U37" s="48">
-        <f t="shared" si="48"/>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="V37" s="48">
-        <f t="shared" si="49"/>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="W37" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X37" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="Y37" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
       <c r="Z37" s="50"/>
@@ -4583,35 +4594,35 @@
         <v>10</v>
       </c>
       <c r="R38" s="48">
-        <f t="shared" si="45"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="S38" s="48">
-        <f t="shared" si="46"/>
+        <f t="shared" si="33"/>
         <v>4</v>
       </c>
       <c r="T38" s="48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="U38" s="48">
-        <f t="shared" si="48"/>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="V38" s="48">
-        <f t="shared" si="49"/>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="W38" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X38" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="Y38" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>11</v>
       </c>
       <c r="AA38" s="54">
@@ -4682,35 +4693,35 @@
         <v>3</v>
       </c>
       <c r="R39" s="48">
-        <f t="shared" si="45"/>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="S39" s="48">
-        <f t="shared" si="46"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="T39" s="48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="U39" s="48">
-        <f t="shared" si="48"/>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="V39" s="48">
-        <f t="shared" si="49"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="W39" s="48">
-        <f t="shared" si="50"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X39" s="46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>9</v>
       </c>
       <c r="Y39" s="46">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>6</v>
       </c>
       <c r="AA39" s="54">
@@ -4759,27 +4770,27 @@
         <v>62</v>
       </c>
       <c r="J40" s="43">
-        <f t="shared" ref="J40:O40" si="51">SUM(J9:J39)</f>
+        <f t="shared" ref="J40:O40" si="40">SUM(J9:J39)</f>
         <v>30</v>
       </c>
       <c r="K40" s="43">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>42</v>
       </c>
       <c r="L40" s="43">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>65</v>
       </c>
       <c r="M40" s="43">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>67</v>
       </c>
       <c r="N40" s="43">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>31</v>
       </c>
       <c r="O40" s="43">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>15</v>
       </c>
       <c r="P40" s="46">
@@ -4791,27 +4802,27 @@
         <v>124</v>
       </c>
       <c r="R40" s="46">
-        <f t="shared" ref="R40:W40" si="52">SUM(B40+J40)</f>
+        <f t="shared" ref="R40:W40" si="41">SUM(B40+J40)</f>
         <v>51</v>
       </c>
       <c r="S40" s="46">
-        <f t="shared" si="52"/>
+        <f t="shared" si="41"/>
         <v>62</v>
       </c>
       <c r="T40" s="46">
-        <f t="shared" si="52"/>
+        <f t="shared" si="41"/>
         <v>99</v>
       </c>
       <c r="U40" s="46">
-        <f t="shared" si="52"/>
+        <f t="shared" si="41"/>
         <v>96</v>
       </c>
       <c r="V40" s="46">
-        <f t="shared" si="52"/>
+        <f t="shared" si="41"/>
         <v>41</v>
       </c>
       <c r="W40" s="46">
-        <f t="shared" si="52"/>
+        <f t="shared" si="41"/>
         <v>28</v>
       </c>
       <c r="X40" s="46">
@@ -4824,7 +4835,7 @@
       </c>
       <c r="AA40" s="60">
         <f>SUM(AA9:AA39)</f>
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="AC40" s="59">
         <f>SUM(AC9:AC39)</f>
@@ -4864,72 +4875,72 @@
     </row>
     <row r="42" spans="1:32" ht="14.25" customHeight="1">
       <c r="A42" s="25"/>
-      <c r="AB42" s="71" t="s">
+      <c r="AB42" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="AC42" s="72"/>
+      <c r="AC42" s="93"/>
       <c r="AD42" s="56">
         <f>SUM(D40+F40+L40+N40)</f>
         <v>140</v>
       </c>
-      <c r="AE42" s="68">
+      <c r="AE42" s="89">
         <f>SUM(AD42+AD43+AD44)</f>
         <v>377</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="14.25" customHeight="1">
       <c r="A43" s="25"/>
-      <c r="AB43" s="71" t="s">
+      <c r="AB43" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="AC43" s="72"/>
+      <c r="AC43" s="93"/>
       <c r="AD43" s="56">
         <f>SUM(E40+G40+M40+O40)</f>
         <v>124</v>
       </c>
-      <c r="AE43" s="68"/>
+      <c r="AE43" s="89"/>
     </row>
     <row r="44" spans="1:32" ht="14.25" customHeight="1">
       <c r="A44" s="25"/>
-      <c r="AB44" s="71" t="s">
+      <c r="AB44" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="AC44" s="72"/>
+      <c r="AC44" s="93"/>
       <c r="AD44" s="56">
         <f>SUM(B40+C40+J40+K40)</f>
         <v>113</v>
       </c>
-      <c r="AE44" s="68"/>
+      <c r="AE44" s="89"/>
     </row>
     <row r="45" spans="1:32" ht="14.25" customHeight="1">
       <c r="P45" s="6"/>
-      <c r="AB45" s="69" t="s">
+      <c r="AB45" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="AC45" s="68"/>
+      <c r="AC45" s="89"/>
       <c r="AD45" s="56">
         <f>SUM(H40+I40)</f>
         <v>127</v>
       </c>
-      <c r="AE45" s="68">
+      <c r="AE45" s="89">
         <f>SUM(H40+I40+P40+Q40)</f>
         <v>377</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="14.25" customHeight="1">
-      <c r="AB46" s="69" t="s">
+      <c r="AB46" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="AC46" s="68"/>
+      <c r="AC46" s="89"/>
       <c r="AD46" s="56">
         <f>SUM(P40+Q40)</f>
         <v>250</v>
       </c>
-      <c r="AE46" s="68"/>
+      <c r="AE46" s="89"/>
     </row>
     <row r="47" spans="1:32" ht="14.25" customHeight="1">
-      <c r="AB47" s="70"/>
-      <c r="AC47" s="70"/>
+      <c r="AB47" s="91"/>
+      <c r="AC47" s="91"/>
       <c r="AD47" s="53"/>
       <c r="AE47" s="53"/>
     </row>
@@ -5893,6 +5904,20 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="AE42:AE44"/>
+    <mergeCell ref="AB45:AC45"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AB42:AC42"/>
+    <mergeCell ref="AB43:AC43"/>
+    <mergeCell ref="AB44:AC44"/>
+    <mergeCell ref="AE45:AE46"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="A4:Y4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A5:Y5"/>
     <mergeCell ref="X7:Y7"/>
     <mergeCell ref="V7:W7"/>
     <mergeCell ref="J6:Q6"/>
@@ -5907,20 +5932,6 @@
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="A4:Y4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A5:Y5"/>
-    <mergeCell ref="AE42:AE44"/>
-    <mergeCell ref="AB45:AC45"/>
-    <mergeCell ref="AB46:AC46"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AB42:AC42"/>
-    <mergeCell ref="AB43:AC43"/>
-    <mergeCell ref="AB44:AC44"/>
-    <mergeCell ref="AE45:AE46"/>
   </mergeCells>
   <pageMargins left="0.70866141732283461" right="0.70866141732283461" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
@@ -9155,115 +9166,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="107"/>
-      <c r="Y1" s="107"/>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="107"/>
-      <c r="AB1" s="107"/>
-      <c r="AC1" s="107"/>
-      <c r="AD1" s="107"/>
-      <c r="AE1" s="107"/>
-      <c r="AF1" s="107"/>
-      <c r="AG1" s="108"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="113"/>
+      <c r="AC1" s="113"/>
+      <c r="AD1" s="113"/>
+      <c r="AE1" s="113"/>
+      <c r="AF1" s="113"/>
+      <c r="AG1" s="114"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" customHeight="1">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="110"/>
-      <c r="X2" s="110"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="110"/>
-      <c r="AA2" s="110"/>
-      <c r="AB2" s="110"/>
-      <c r="AC2" s="110"/>
-      <c r="AD2" s="110"/>
-      <c r="AE2" s="110"/>
-      <c r="AF2" s="110"/>
-      <c r="AG2" s="111"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="116"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="116"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="116"/>
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="117"/>
     </row>
     <row r="3" spans="1:34">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="112" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
-      <c r="AB3" s="107"/>
-      <c r="AC3" s="107"/>
-      <c r="AD3" s="107"/>
-      <c r="AE3" s="107"/>
-      <c r="AF3" s="107"/>
-      <c r="AG3" s="108"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
+      <c r="R3" s="113"/>
+      <c r="S3" s="113"/>
+      <c r="T3" s="113"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="113"/>
+      <c r="Y3" s="113"/>
+      <c r="Z3" s="113"/>
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113"/>
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="113"/>
+      <c r="AE3" s="113"/>
+      <c r="AF3" s="113"/>
+      <c r="AG3" s="114"/>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" s="57" t="s">
@@ -9370,40 +9381,40 @@
       <c r="A5" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="113"/>
-      <c r="N5" s="113"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="113"/>
-      <c r="T5" s="113"/>
-      <c r="U5" s="113"/>
-      <c r="V5" s="113"/>
-      <c r="W5" s="113"/>
-      <c r="X5" s="113"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="114"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="109"/>
+      <c r="Z5" s="109"/>
+      <c r="AA5" s="109"/>
+      <c r="AB5" s="109"/>
+      <c r="AC5" s="109"/>
+      <c r="AD5" s="109"/>
+      <c r="AE5" s="109"/>
+      <c r="AF5" s="109"/>
+      <c r="AG5" s="110"/>
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="61">
@@ -9485,10 +9496,10 @@
       </c>
     </row>
     <row r="7" spans="1:34">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="57">
         <v>0</v>
       </c>
@@ -9616,39 +9627,39 @@
       <c r="A8" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-      <c r="T8" s="116"/>
-      <c r="U8" s="116"/>
-      <c r="V8" s="116"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="116"/>
-      <c r="AA8" s="116"/>
-      <c r="AB8" s="116"/>
-      <c r="AC8" s="116"/>
-      <c r="AD8" s="116"/>
-      <c r="AE8" s="116"/>
-      <c r="AF8" s="116"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="111"/>
+      <c r="N8" s="111"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+      <c r="T8" s="111"/>
+      <c r="U8" s="111"/>
+      <c r="V8" s="111"/>
+      <c r="W8" s="111"/>
+      <c r="X8" s="111"/>
+      <c r="Y8" s="111"/>
+      <c r="Z8" s="111"/>
+      <c r="AA8" s="111"/>
+      <c r="AB8" s="111"/>
+      <c r="AC8" s="111"/>
+      <c r="AD8" s="111"/>
+      <c r="AE8" s="111"/>
+      <c r="AF8" s="111"/>
       <c r="AG8" s="64"/>
       <c r="AH8" s="35">
         <f t="shared" ref="AH8:AH67" si="1">SUM(C8:AG8)</f>
@@ -9836,10 +9847,10 @@
       </c>
     </row>
     <row r="13" spans="1:34">
-      <c r="A13" s="115" t="s">
+      <c r="A13" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="115"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="57">
         <f>SUM(C9:C12)</f>
         <v>0</v>
@@ -9969,40 +9980,40 @@
       <c r="A14" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="112" t="s">
+      <c r="B14" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="113"/>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="113"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="113"/>
-      <c r="T14" s="113"/>
-      <c r="U14" s="113"/>
-      <c r="V14" s="113"/>
-      <c r="W14" s="113"/>
-      <c r="X14" s="113"/>
-      <c r="Y14" s="113"/>
-      <c r="Z14" s="113"/>
-      <c r="AA14" s="113"/>
-      <c r="AB14" s="113"/>
-      <c r="AC14" s="113"/>
-      <c r="AD14" s="113"/>
-      <c r="AE14" s="113"/>
-      <c r="AF14" s="113"/>
-      <c r="AG14" s="114"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="109"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="109"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="109"/>
+      <c r="S14" s="109"/>
+      <c r="T14" s="109"/>
+      <c r="U14" s="109"/>
+      <c r="V14" s="109"/>
+      <c r="W14" s="109"/>
+      <c r="X14" s="109"/>
+      <c r="Y14" s="109"/>
+      <c r="Z14" s="109"/>
+      <c r="AA14" s="109"/>
+      <c r="AB14" s="109"/>
+      <c r="AC14" s="109"/>
+      <c r="AD14" s="109"/>
+      <c r="AE14" s="109"/>
+      <c r="AF14" s="109"/>
+      <c r="AG14" s="110"/>
       <c r="AH14" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -10279,10 +10290,10 @@
       </c>
     </row>
     <row r="21" spans="1:34">
-      <c r="A21" s="115" t="s">
+      <c r="A21" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="115"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="57">
         <f>SUM(C18:C20)</f>
         <v>0</v>
@@ -10412,40 +10423,40 @@
       <c r="A22" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="112" t="s">
+      <c r="B22" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="113"/>
-      <c r="D22" s="113"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="113"/>
-      <c r="G22" s="113"/>
-      <c r="H22" s="113"/>
-      <c r="I22" s="113"/>
-      <c r="J22" s="113"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="113"/>
-      <c r="N22" s="113"/>
-      <c r="O22" s="113"/>
-      <c r="P22" s="113"/>
-      <c r="Q22" s="113"/>
-      <c r="R22" s="113"/>
-      <c r="S22" s="113"/>
-      <c r="T22" s="113"/>
-      <c r="U22" s="113"/>
-      <c r="V22" s="113"/>
-      <c r="W22" s="113"/>
-      <c r="X22" s="113"/>
-      <c r="Y22" s="113"/>
-      <c r="Z22" s="113"/>
-      <c r="AA22" s="113"/>
-      <c r="AB22" s="113"/>
-      <c r="AC22" s="113"/>
-      <c r="AD22" s="113"/>
-      <c r="AE22" s="113"/>
-      <c r="AF22" s="113"/>
-      <c r="AG22" s="114"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="109"/>
+      <c r="M22" s="109"/>
+      <c r="N22" s="109"/>
+      <c r="O22" s="109"/>
+      <c r="P22" s="109"/>
+      <c r="Q22" s="109"/>
+      <c r="R22" s="109"/>
+      <c r="S22" s="109"/>
+      <c r="T22" s="109"/>
+      <c r="U22" s="109"/>
+      <c r="V22" s="109"/>
+      <c r="W22" s="109"/>
+      <c r="X22" s="109"/>
+      <c r="Y22" s="109"/>
+      <c r="Z22" s="109"/>
+      <c r="AA22" s="109"/>
+      <c r="AB22" s="109"/>
+      <c r="AC22" s="109"/>
+      <c r="AD22" s="109"/>
+      <c r="AE22" s="109"/>
+      <c r="AF22" s="109"/>
+      <c r="AG22" s="110"/>
       <c r="AH22" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -10603,10 +10614,10 @@
       </c>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="115"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="57">
         <f>SUM(C23:C25)</f>
         <v>0</v>
@@ -10966,10 +10977,10 @@
       </c>
     </row>
     <row r="32" spans="1:34">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="115"/>
+      <c r="B32" s="107"/>
       <c r="C32" s="57">
         <f>SUM(C28:C31)</f>
         <v>0</v>
@@ -11327,10 +11338,10 @@
       </c>
     </row>
     <row r="38" spans="1:34">
-      <c r="A38" s="115" t="s">
+      <c r="A38" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="115"/>
+      <c r="B38" s="107"/>
       <c r="C38" s="57">
         <f>SUM(C34:C37)</f>
         <v>0</v>
@@ -11460,40 +11471,40 @@
       <c r="A39" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="112" t="s">
+      <c r="B39" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="113"/>
-      <c r="D39" s="113"/>
-      <c r="E39" s="113"/>
-      <c r="F39" s="113"/>
-      <c r="G39" s="113"/>
-      <c r="H39" s="113"/>
-      <c r="I39" s="113"/>
-      <c r="J39" s="113"/>
-      <c r="K39" s="113"/>
-      <c r="L39" s="113"/>
-      <c r="M39" s="113"/>
-      <c r="N39" s="113"/>
-      <c r="O39" s="113"/>
-      <c r="P39" s="113"/>
-      <c r="Q39" s="113"/>
-      <c r="R39" s="113"/>
-      <c r="S39" s="113"/>
-      <c r="T39" s="113"/>
-      <c r="U39" s="113"/>
-      <c r="V39" s="113"/>
-      <c r="W39" s="113"/>
-      <c r="X39" s="113"/>
-      <c r="Y39" s="113"/>
-      <c r="Z39" s="113"/>
-      <c r="AA39" s="113"/>
-      <c r="AB39" s="113"/>
-      <c r="AC39" s="113"/>
-      <c r="AD39" s="113"/>
-      <c r="AE39" s="113"/>
-      <c r="AF39" s="113"/>
-      <c r="AG39" s="114"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="109"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="109"/>
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
+      <c r="N39" s="109"/>
+      <c r="O39" s="109"/>
+      <c r="P39" s="109"/>
+      <c r="Q39" s="109"/>
+      <c r="R39" s="109"/>
+      <c r="S39" s="109"/>
+      <c r="T39" s="109"/>
+      <c r="U39" s="109"/>
+      <c r="V39" s="109"/>
+      <c r="W39" s="109"/>
+      <c r="X39" s="109"/>
+      <c r="Y39" s="109"/>
+      <c r="Z39" s="109"/>
+      <c r="AA39" s="109"/>
+      <c r="AB39" s="109"/>
+      <c r="AC39" s="109"/>
+      <c r="AD39" s="109"/>
+      <c r="AE39" s="109"/>
+      <c r="AF39" s="109"/>
+      <c r="AG39" s="110"/>
       <c r="AH39" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -11801,10 +11812,10 @@
       </c>
     </row>
     <row r="47" spans="1:34">
-      <c r="A47" s="115" t="s">
+      <c r="A47" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="115"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="57">
         <f>SUM(C40:C46)</f>
         <v>0</v>
@@ -11935,40 +11946,40 @@
       <c r="A48" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="112" t="s">
+      <c r="B48" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="113"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="113"/>
-      <c r="F48" s="113"/>
-      <c r="G48" s="113"/>
-      <c r="H48" s="113"/>
-      <c r="I48" s="113"/>
-      <c r="J48" s="113"/>
-      <c r="K48" s="113"/>
-      <c r="L48" s="113"/>
-      <c r="M48" s="113"/>
-      <c r="N48" s="113"/>
-      <c r="O48" s="113"/>
-      <c r="P48" s="113"/>
-      <c r="Q48" s="113"/>
-      <c r="R48" s="113"/>
-      <c r="S48" s="113"/>
-      <c r="T48" s="113"/>
-      <c r="U48" s="113"/>
-      <c r="V48" s="113"/>
-      <c r="W48" s="113"/>
-      <c r="X48" s="113"/>
-      <c r="Y48" s="113"/>
-      <c r="Z48" s="113"/>
-      <c r="AA48" s="113"/>
-      <c r="AB48" s="113"/>
-      <c r="AC48" s="113"/>
-      <c r="AD48" s="113"/>
-      <c r="AE48" s="113"/>
-      <c r="AF48" s="113"/>
-      <c r="AG48" s="114"/>
+      <c r="C48" s="109"/>
+      <c r="D48" s="109"/>
+      <c r="E48" s="109"/>
+      <c r="F48" s="109"/>
+      <c r="G48" s="109"/>
+      <c r="H48" s="109"/>
+      <c r="I48" s="109"/>
+      <c r="J48" s="109"/>
+      <c r="K48" s="109"/>
+      <c r="L48" s="109"/>
+      <c r="M48" s="109"/>
+      <c r="N48" s="109"/>
+      <c r="O48" s="109"/>
+      <c r="P48" s="109"/>
+      <c r="Q48" s="109"/>
+      <c r="R48" s="109"/>
+      <c r="S48" s="109"/>
+      <c r="T48" s="109"/>
+      <c r="U48" s="109"/>
+      <c r="V48" s="109"/>
+      <c r="W48" s="109"/>
+      <c r="X48" s="109"/>
+      <c r="Y48" s="109"/>
+      <c r="Z48" s="109"/>
+      <c r="AA48" s="109"/>
+      <c r="AB48" s="109"/>
+      <c r="AC48" s="109"/>
+      <c r="AD48" s="109"/>
+      <c r="AE48" s="109"/>
+      <c r="AF48" s="109"/>
+      <c r="AG48" s="110"/>
     </row>
     <row r="49" spans="1:34">
       <c r="A49" s="57">
@@ -12337,10 +12348,10 @@
       </c>
     </row>
     <row r="57" spans="1:34">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="115"/>
+      <c r="B57" s="107"/>
       <c r="C57" s="57">
         <f>SUM(C49:C56)</f>
         <v>0</v>
@@ -12470,40 +12481,40 @@
       <c r="A58" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="112" t="s">
+      <c r="B58" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="113"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="113"/>
-      <c r="F58" s="113"/>
-      <c r="G58" s="113"/>
-      <c r="H58" s="113"/>
-      <c r="I58" s="113"/>
-      <c r="J58" s="113"/>
-      <c r="K58" s="113"/>
-      <c r="L58" s="113"/>
-      <c r="M58" s="113"/>
-      <c r="N58" s="113"/>
-      <c r="O58" s="113"/>
-      <c r="P58" s="113"/>
-      <c r="Q58" s="113"/>
-      <c r="R58" s="113"/>
-      <c r="S58" s="113"/>
-      <c r="T58" s="113"/>
-      <c r="U58" s="113"/>
-      <c r="V58" s="113"/>
-      <c r="W58" s="113"/>
-      <c r="X58" s="113"/>
-      <c r="Y58" s="113"/>
-      <c r="Z58" s="113"/>
-      <c r="AA58" s="113"/>
-      <c r="AB58" s="113"/>
-      <c r="AC58" s="113"/>
-      <c r="AD58" s="113"/>
-      <c r="AE58" s="113"/>
-      <c r="AF58" s="113"/>
-      <c r="AG58" s="114"/>
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="109"/>
+      <c r="F58" s="109"/>
+      <c r="G58" s="109"/>
+      <c r="H58" s="109"/>
+      <c r="I58" s="109"/>
+      <c r="J58" s="109"/>
+      <c r="K58" s="109"/>
+      <c r="L58" s="109"/>
+      <c r="M58" s="109"/>
+      <c r="N58" s="109"/>
+      <c r="O58" s="109"/>
+      <c r="P58" s="109"/>
+      <c r="Q58" s="109"/>
+      <c r="R58" s="109"/>
+      <c r="S58" s="109"/>
+      <c r="T58" s="109"/>
+      <c r="U58" s="109"/>
+      <c r="V58" s="109"/>
+      <c r="W58" s="109"/>
+      <c r="X58" s="109"/>
+      <c r="Y58" s="109"/>
+      <c r="Z58" s="109"/>
+      <c r="AA58" s="109"/>
+      <c r="AB58" s="109"/>
+      <c r="AC58" s="109"/>
+      <c r="AD58" s="109"/>
+      <c r="AE58" s="109"/>
+      <c r="AF58" s="109"/>
+      <c r="AG58" s="110"/>
       <c r="AH58" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -12941,10 +12952,10 @@
       </c>
     </row>
     <row r="68" spans="1:40">
-      <c r="A68" s="115" t="s">
+      <c r="A68" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="115"/>
+      <c r="B68" s="107"/>
       <c r="C68" s="61">
         <f>SUM(C59:C67)</f>
         <v>0</v>
@@ -13071,10 +13082,10 @@
       </c>
     </row>
     <row r="69" spans="1:40" ht="15.6">
-      <c r="A69" s="117" t="s">
+      <c r="A69" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="117"/>
+      <c r="B69" s="106"/>
       <c r="C69" s="61">
         <f>SUM(C7+C13+C21+C26+C32+C38+C47+C57+C68)</f>
         <v>0</v>
@@ -13212,6 +13223,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="A2:AG2"/>
+    <mergeCell ref="B5:AG5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A3:AG3"/>
+    <mergeCell ref="B8:AF8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A38:B38"/>
@@ -13222,16 +13243,6 @@
     <mergeCell ref="B48:AG48"/>
     <mergeCell ref="B58:AG58"/>
     <mergeCell ref="A57:B57"/>
-    <mergeCell ref="B8:AF8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="A2:AG2"/>
-    <mergeCell ref="B5:AG5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A3:AG3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="7" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>